<commit_message>
update prompt & subsequent run
</commit_message>
<xml_diff>
--- a/ground-truths-list/data/02_intermediate/structured_contraindications_list.xlsx
+++ b/ground-truths-list/data/02_intermediate/structured_contraindications_list.xlsx
@@ -492,7 +492,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['diabetic ketoacidosis']</t>
+          <t>['diabetic ketoacidosis', 'Type I diabetes']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -560,7 +560,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['dehydrated azotemic patients']</t>
+          <t>['dehydration with azotemia']</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['hepatitis', 'cirrhosis']</t>
+          <t>['Active hepatic disease', 'Cirrhosis', 'Hepatitis']</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -594,7 +594,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>['Diabetes insipidus', 'Severe renal impairment', 'Severe cardiovascular disease', 'Bradycardia', 'Hypothyroidism', 'Myasthenia gravis', 'Parkinson's disease', 'Dehydration', 'Sodium depletion', 'Hypovolemia', 'Pregnant women', 'Breastfeeding women', 'Children under 12 years of age']</t>
+          <t>['Diabetes insipidus', 'Severe renal impairment', 'Severe cardiovascular disease', 'Hypothyroidism', 'Dehydration', 'Sodium depletion', 'Bradycardia', 'Myocardial infarction', 'Stroke', 'Congestive heart failure', 'Hypertension', 'Arrhythmias', 'Edema', 'Gastrointestinal bleeding', 'Renal failure', 'Hepatic failure', 'Hypokalemia', 'Hypomagnesemia', 'Hypocalcemia', 'Hyperparathyroidism', 'Addison's disease', 'Cushing's syndrome', 'Pheochromocytoma', 'Myasthenia gravis', 'Parkinson's disease', 'Multiple sclerosis', 'Huntington's disease', 'Alzheimer's disease', 'Dementia', 'Epilepsy', 'Seizures', 'Headache', 'Dizziness', 'Tremor', 'Fatigue', 'Weight gain', 'Nausea', 'Vomiting', 'Diarrhea', 'Constipation', 'Polyuria', 'Polydipsia', 'Alopecia', 'Acne', 'Rash', 'Pruritis', 'Photosensitivity', 'Hypothyroidism', 'Hyperthyroidism', 'Goiter', 'Hypoparathyroidism', 'Hyperparathyroidism', 'Hypokalemia', 'Hyperkalemia', 'Hypomagnesemia', 'Hypermagnesemia', 'Hypocalcemia', 'Hypercalcemia', 'Hypoglycemia', 'Hyperglycemia', 'Diabetes mellitus', 'Hypophosphatemia', 'Hyperphosphatemia', 'Hypoalbuminemia', 'Hyperalbuminemia', 'Hypoproteinemia', 'Hyperproteinemia', 'Anemia', 'Leukopenia', 'Thrombocytopenia', 'Neutropenia', 'Agranulocytosis', 'Aplastic anemia', 'Hemolytic anemia', 'Pancytopenia', 'Eosinophilia', 'Lymphadenopathy', 'Splenomegaly', 'Hepatitis', 'Cirrhosis', 'Nephritis', 'Nephrosis', 'Nephrotic syndrome', 'Glomerulonephritis', 'Interstitial nephritis', 'Pyelonephritis', 'Cystitis', 'Urethritis', 'Prostatitis', 'Epididymitis', 'Orchitis', 'Salpingitis', 'Oophoritis', 'Endometritis', 'Cervicitis', 'Vaginitis', 'Balanitis', 'Posthitis', 'Syphilis', 'Gonorrhea', 'Chlamydia', 'Herpes simplex', 'Genital warts', 'Human papillomavirus', 'Candidiasis', 'Trichomoniasis', 'Bacterial vaginosis', 'Pelvic inflammatory disease', 'Pneumonia', 'Bronchitis', 'Asthma', 'Chronic obstructive pulmonary disease', 'Pulmonary embolism', 'Deep vein thrombosis', 'Myocardial infarction', 'Stroke', 'Cerebrovascular accident', 'Transient ischemic attack', 'Angina pectoris', 'Heart failure', 'Arrhythmias', 'Hypertension', 'Hypotension', 'Peripheral vascular disease', 'Atherosclerosis', 'Hyperlipidemia', 'Dyslipidemia', 'Diabetes mellitus', 'Obesity', 'Metabolic syndrome', 'Gastroesophageal reflux disease', 'Peptic ulcer disease', 'Gastritis', 'Duodenitis', 'Colitis', 'Crohn's disease', 'Ulcerative colitis', 'Irritable bowel syndrome', 'Constipation', 'Diarrhea', 'Hemorrhoids', 'Anal fissure', 'Fissure-in-ano', 'Abscess', 'Fistula', 'Perianal abscess', 'Perianal fistula', 'Pancreatitis', 'Cholecystitis', 'Cholelithiasis', 'Gallstones', 'Hepatitis', 'Cirrhosis', 'Hepatic encephalopathy', 'Ascites', 'Jaundice', 'Splenomegaly', 'Hepatomegaly', 'Kidney failure', 'Renal failure', 'Acute kidney injury', 'Chronic kidney disease', 'End-stage renal disease', 'Urinary tract infection', 'Cystitis', 'Urethritis', 'Prostatitis', 'Epididymitis', 'Orchitis', 'Salpingitis', 'Oophoritis', 'Endometritis', 'Cervicitis', 'Vaginitis', 'Balanitis', 'Posthitis', 'Syphilis', 'Gonorrhea', 'Chlamydia', 'Herpes simplex', 'Genital warts', 'Human papillomavirus', 'Candidiasis', 'Trichomoniasis', 'Bacterial vaginosis', 'Pelvic inflammatory disease', 'Osteoporosis', 'Osteomalacia', 'Rickets', 'Gout', 'Pseudogout', 'Rheumatoid arthritis', 'Osteoarthritis', 'Lupus', 'Scleroderma', 'Sjögren's syndrome', 'Polymyositis', 'Dermatomyositis', 'Vasculitis', 'Myasthenia gravis', 'Multiple sclerosis', 'Parkinson's disease', 'Alzheimer's disease', 'Dementia', 'Epilepsy', 'Seizures',</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -743,7 +743,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>['corn allergy']</t>
+          <t>['Corn allergy']</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>['trichomoniasis during the first trimester of pregnancy']</t>
+          <t>['trichomoniasis']</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>['Acute myocardial infarction', 'Septicemia', 'Congestive heart failure', 'Diabetic ketoacidosis', 'Acute alteration of renal function']</t>
+          <t>['Acute myocardial infarction', 'Septicemia', 'Congestive heart failure', 'Diabetic ketoacidosis', 'Acute or chronic metabolic acidosis']</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1185,7 +1185,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>NO LLM OUTPUT</t>
+          <t>['active peptic ulcer disease', 'recent gastrointestinal bleeding', 'gastrointestinal perforation', 'advanced renal impairment', 'risk for renal failure due to volume depletion', 'labor and delivery', 'cerebrovascular bleeding', 'hemorrhagic diathesis', 'incomplete hemostasis', 'high risk of bleeding']</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1287,7 +1287,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>['Clinically significant sensitivity to leucovorin', 'Clinically significant sensitivity to methotrexate']</t>
+          <t>['clinically significant sensitivity to leucovorin', 'clinically significant sensitivity to methotrexate']</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>['asthma', 'urticaria', 'allergic-type reactions after taking aspirin or other NSAIDs']</t>
+          <t>['asthma', 'urticaria', 'allergic-type reactions after taking aspirin or other NSAIDs', 'anaphylactic-like reactions']</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>['diagnostic/contrast/radiolabel']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1644,7 +1644,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>['Pregnancy', 'Breastfeeding', 'Women of childbearing potential unless they fulfill all requirements of the iPLEDGE program']</t>
+          <t>['Pregnancy', 'Breastfeeding', 'Women of childbearing potential unless all conditions of the iPLEDGE program are met']</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1678,7 +1678,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>NO LLM OUTPUT</t>
+          <t>['bronchial asthma', 'sinus bradycardia', 'second and third degree AV block', 'congenital or acquired long QT syndromes', 'cardiogenic shock', 'uncontrolled heart failure']</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>['fetal abnormalities']</t>
+          <t>['early pregnancy']</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>['Carcinoma of the breast in males', 'Carcinoma of the prostate', 'Carcinoma of the breast in females with hypercalcemia', 'Pregnancy', 'Nephrosis', 'Nephritic phase of nephritis']</t>
+          <t>['Carcinoma of the breast in males', 'Carcinoma of the prostate', 'Carcinoma of the breast in females with hypercalcemia', 'Pregnancy', 'Nephrosis', 'Nephrotic phase of nephritis']</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2086,7 +2086,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['sensitivity reactions to any of its components']</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">

</xml_diff>